<commit_message>
Add frame change to ipacheckids
</commit_message>
<xml_diff>
--- a/folders/04_checks/02_outputs/hfc_outputs.xlsx
+++ b/folders/04_checks/02_outputs/hfc_outputs.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="120">
   <si>
     <t>serial</t>
   </si>
@@ -298,6 +298,66 @@
   </si>
   <si>
     <t>uuid:faddd692-de86-11e8-9f32-f2801f111128</t>
+  </si>
+  <si>
+    <t>uuid:2b2763e1-71b6-4e1e-8023-c15cdf7fa39d</t>
+  </si>
+  <si>
+    <t>uuid:faded75e-de86-11e8-9f32-f2801f194957</t>
+  </si>
+  <si>
+    <t>Differences</t>
+  </si>
+  <si>
+    <t>Total Compared</t>
+  </si>
+  <si>
+    <t>Percent Difference</t>
+  </si>
+  <si>
+    <t>serial</t>
+  </si>
+  <si>
+    <t>submissiondate</t>
+  </si>
+  <si>
+    <t>20nov2015</t>
+  </si>
+  <si>
+    <t>19nov2015</t>
+  </si>
+  <si>
+    <t>23dec2015</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>1201</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>enumid</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>uuid:faddd692-de86-11e8-9f32-f2801f111128</t>
+  </si>
+  <si>
+    <t>uuid:fade4d02-de86-11e8-9f32-f2801f197841</t>
   </si>
   <si>
     <t>uuid:2b2763e1-71b6-4e1e-8023-c15cdf7fa39d</t>
@@ -363,28 +423,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="C1" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="E1" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="F1" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="G1" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="H1" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2">
@@ -392,16 +452,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="E2" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
@@ -418,16 +478,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="F3" s="1">
         <v>7</v>
@@ -444,16 +504,16 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -470,16 +530,16 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
       <c r="E5" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="F5" s="1">
         <v>22</v>

</xml_diff>